<commit_message>
enviar status e tabela de eventos
</commit_message>
<xml_diff>
--- a/Eventos/nova tabela/Eventos.xlsx
+++ b/Eventos/nova tabela/Eventos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1800560\Desktop\OPE\Eventos\nova tabela\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1800794\Desktop\OPE\Eventos\nova tabela\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -168,7 +168,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -243,12 +243,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF7030A0"/>
+        <fgColor rgb="FF2AEE4F"/>
         <bgColor rgb="FFFAA61A"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF6187DD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -272,15 +278,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
@@ -290,109 +287,7 @@
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -412,20 +307,120 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
-      <right/>
-      <top/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -448,16 +443,49 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -469,51 +497,40 @@
     <xf numFmtId="0" fontId="13" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -538,6 +555,15 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF6187DD"/>
+      <color rgb="FF2AEE4F"/>
+      <color rgb="FFFF5DAE"/>
+      <color rgb="FFCC0066"/>
+      <color rgb="FFFF66CC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -812,10 +838,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -830,123 +856,135 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="56.65" customHeight="1" thickBot="1">
-      <c r="A1" s="15"/>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
+      <c r="A1" s="6"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16" t="s">
+      <c r="F1" s="5"/>
+      <c r="G1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="2"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="7"/>
     </row>
     <row r="2" spans="1:10" ht="56.65" customHeight="1" thickBot="1">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="13"/>
+      <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="56.65" customHeight="1" thickBot="1">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="32"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="21"/>
+    </row>
+    <row r="4" spans="1:10" ht="56.65" customHeight="1">
+      <c r="A4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B4" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C4" s="16">
         <v>1</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D4" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7" t="s">
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="7"/>
-      <c r="J3" s="8"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="21"/>
     </row>
-    <row r="4" spans="1:10" ht="56.65" customHeight="1" thickBot="1">
-      <c r="A4" s="18"/>
-      <c r="B4" s="20"/>
-      <c r="C4" s="9">
+    <row r="5" spans="1:10" ht="56.65" customHeight="1" thickBot="1">
+      <c r="A5" s="11"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="17">
         <v>2</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D5" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="12" t="s">
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="13"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="25"/>
     </row>
-    <row r="5" spans="1:10" ht="88.5" customHeight="1" thickBot="1">
-      <c r="A5" s="25" t="s">
+    <row r="6" spans="1:10" ht="88.5" customHeight="1" thickBot="1">
+      <c r="A6" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="19">
+      <c r="C6" s="26">
         <v>3</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D6" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11" t="s">
+      <c r="E6" s="28"/>
+      <c r="F6" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="13"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="30"/>
     </row>
-    <row r="6" spans="1:10" ht="15.75">
-      <c r="A6" s="22"/>
-      <c r="B6" s="24"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="14"/>
+    <row r="7" spans="1:10" ht="15.75">
+      <c r="A7" s="3"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="2"/>
     </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="21"/>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
+    <row r="8" spans="1:10">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -954,8 +992,8 @@
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0.39370078740157477" bottom="0.39370078740157477" header="0" footer="0"/>
   <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
tabela eventos atualizada cronologicamente
</commit_message>
<xml_diff>
--- a/Eventos/nova tabela/Eventos.xlsx
+++ b/Eventos/nova tabela/Eventos.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="foco" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>Externo</t>
   </si>
@@ -63,9 +63,6 @@
     <t>Funcionário verifica materiais</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
     <t>Funcionário realiza reparo</t>
   </si>
   <si>
@@ -78,7 +75,31 @@
     <t>x</t>
   </si>
   <si>
-    <t>Verificar detalhes do reparo</t>
+    <t>Registrar ordem de serviço</t>
+  </si>
+  <si>
+    <t>Funcionário registra ordem de serviço</t>
+  </si>
+  <si>
+    <t>Realizar atendimento ao cliente</t>
+  </si>
+  <si>
+    <t>Cliente confirma orçamento</t>
+  </si>
+  <si>
+    <t>x(2)</t>
+  </si>
+  <si>
+    <t>Cliente solicita atendimento</t>
+  </si>
+  <si>
+    <t>X(3)</t>
+  </si>
+  <si>
+    <t>Atendente verifica status para enviar ao cliente.</t>
+  </si>
+  <si>
+    <t>x(4)</t>
   </si>
 </sst>
 </file>
@@ -168,7 +189,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -253,8 +274,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF5D5D"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -420,6 +447,32 @@
       </top>
       <bottom style="medium">
         <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -443,7 +496,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -455,83 +508,89 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="17">
@@ -557,11 +616,12 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
-      <color rgb="FF6187DD"/>
-      <color rgb="FF2AEE4F"/>
+      <color rgb="FFFF5D5D"/>
       <color rgb="FFFF5DAE"/>
       <color rgb="FFCC0066"/>
       <color rgb="FFFF66CC"/>
+      <color rgb="FF6187DD"/>
+      <color rgb="FF2AEE4F"/>
     </mruColors>
   </colors>
   <extLst>
@@ -838,10 +898,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -856,26 +916,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="56.65" customHeight="1" thickBot="1">
-      <c r="A1" s="6"/>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
+      <c r="A1" s="22"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5" t="s">
+      <c r="F1" s="23"/>
+      <c r="G1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="7"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="5"/>
     </row>
     <row r="2" spans="1:10" ht="56.65" customHeight="1" thickBot="1">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="13"/>
+      <c r="B2" s="25"/>
       <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
@@ -901,99 +961,151 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="56.65" customHeight="1" thickBot="1">
-      <c r="A3" s="32"/>
-      <c r="B3" s="31"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="21"/>
+    <row r="3" spans="1:10" ht="69.95" customHeight="1" thickBot="1">
+      <c r="A3" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="8">
+        <v>1</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="12"/>
     </row>
-    <row r="4" spans="1:10" ht="56.65" customHeight="1">
-      <c r="A4" s="10" t="s">
+    <row r="4" spans="1:10" ht="69.95" customHeight="1" thickBot="1">
+      <c r="A4" s="34"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="8">
+        <v>2</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="10"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="12"/>
+    </row>
+    <row r="5" spans="1:10" ht="69.95" customHeight="1" thickBot="1">
+      <c r="A5" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="8">
+        <v>3</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="12"/>
+    </row>
+    <row r="6" spans="1:10" ht="56.65" customHeight="1" thickBot="1">
+      <c r="A6" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B6" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="16">
-        <v>1</v>
-      </c>
-      <c r="D4" s="18" t="s">
+      <c r="C6" s="8">
+        <v>4</v>
+      </c>
+      <c r="D6" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20" t="s">
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="12"/>
+    </row>
+    <row r="7" spans="1:10" ht="56.65" customHeight="1" thickBot="1">
+      <c r="A7" s="27"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="8">
+        <v>5</v>
+      </c>
+      <c r="D7" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="20"/>
-      <c r="J4" s="21"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="16"/>
     </row>
-    <row r="5" spans="1:10" ht="56.65" customHeight="1" thickBot="1">
-      <c r="A5" s="11"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="17">
-        <v>2</v>
-      </c>
-      <c r="D5" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="24" t="s">
+    <row r="8" spans="1:10" ht="88.5" customHeight="1" thickBot="1">
+      <c r="A8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="24"/>
-      <c r="I5" s="24"/>
-      <c r="J5" s="25"/>
+      <c r="B8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="8">
+        <v>6</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="20"/>
     </row>
-    <row r="6" spans="1:10" ht="88.5" customHeight="1" thickBot="1">
-      <c r="A6" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="26">
-        <v>3</v>
-      </c>
-      <c r="D6" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="29"/>
-      <c r="H6" s="29"/>
-      <c r="I6" s="29"/>
-      <c r="J6" s="30"/>
+    <row r="9" spans="1:10" ht="15.75">
+      <c r="A9" s="3"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="2"/>
     </row>
-    <row r="7" spans="1:10" ht="15.75">
-      <c r="A7" s="3"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
+    <row r="10" spans="1:10">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="8">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0.39370078740157477" bottom="0.39370078740157477" header="0" footer="0"/>
   <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>